<commit_message>
Modificación Listado, objetivo y cronograma.
</commit_message>
<xml_diff>
--- a/Anteproyectos2021/Cronograma&Presupuesto/Actividades&Cronograma31052021.xlsx
+++ b/Anteproyectos2021/Cronograma&Presupuesto/Actividades&Cronograma31052021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma_1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="182">
   <si>
     <t>OBJETIVOS</t>
   </si>
@@ -389,21 +389,12 @@
     <t>Comparación de los resultados obtenidos con el algoritmo de Matlab con el Listado de tipos de daños y condiciones más frecuentes.</t>
   </si>
   <si>
-    <t>Listado de tipos de daños o condiciones más frecuentes.</t>
-  </si>
-  <si>
-    <t>Técnicas de procesamiento de imágenes más comunes para identificar formas u objetos en imágenes termográficas de paneles fotovoltaicos.</t>
-  </si>
-  <si>
     <t>Desarrollo de pruebas de las técnicas de procesamiento de imágenes termográficas más comunes con Matlab.</t>
   </si>
   <si>
     <t>Identificación de la técnica de procesamiento de imágenes.</t>
   </si>
   <si>
-    <t>Listado de resultados de las técnicas más comunes.</t>
-  </si>
-  <si>
     <t>Desarrollar pruebas de asociación entre Matlab y el listado de imágenes de los tipos de daños o condiciones más frecuentes.</t>
   </si>
   <si>
@@ -416,69 +407,30 @@
     <t>Implementación de un algoritmo en Matlab de acuerdo al modelo establecido previamente.</t>
   </si>
   <si>
-    <t>Determinación de condición de un panel fotovoltaico a partir de imagen termografica previamente verificada.</t>
-  </si>
-  <si>
-    <t>Investigación sobre escenarios más comunes para la captura de imágenes termografica a paneles fotovoltaicos.</t>
-  </si>
-  <si>
-    <t>Listado de condiciones de captura de imágenes para la ejecución del algoritmo.</t>
-  </si>
-  <si>
     <t>Diseño de un modelo de ensayo para el algoritmo desarrollado.</t>
   </si>
   <si>
-    <t>Modelo de ensayo para el algoritmo desarrollado a partir de las condiciones de captura.</t>
-  </si>
-  <si>
     <t>Ejecución del algoritmo desarrollado mediante el modelo de ensayo.</t>
   </si>
   <si>
-    <t>Resultados de algoritmos; detección de condición de un panel fotovoltaico a parir de una imagen termográfica.</t>
-  </si>
-  <si>
     <t>Verificación de los resultados obtenidos.</t>
   </si>
   <si>
-    <t>Conclusión de la prueba realizada.</t>
-  </si>
-  <si>
-    <t>Algoritmo de procesamiento de imágenes  termográficas en Matlab.</t>
-  </si>
-  <si>
-    <t>Tipos  de daños o condiciones observados en los paneles solares mediante imágenes termográficas.</t>
-  </si>
-  <si>
     <t>Desarrollo de un listado de los tipos daño y condiciones más frecuentes observados en las imágenes termográfica de paneles fotovoltaicos.</t>
   </si>
   <si>
-    <t>Relación de las formas u objetos obtenidos en el procesamiento de imágenes termográficas en Matlab con el listado de tipos de daños o condiciones más frecuentes.</t>
-  </si>
-  <si>
     <t>Investigación sobre almacenamiento de información en Matlab para la respectiva construcción de conjunto de imágenes.</t>
   </si>
   <si>
-    <t>Definición almacenamiento de datos en Matlab.</t>
-  </si>
-  <si>
     <t>Implementación de un algoritmo de asociación entre el conjunto de imágenes y Matlab.</t>
   </si>
   <si>
-    <t>Algoritmo de asociación de imágenes tipificadas con Matlab.</t>
-  </si>
-  <si>
-    <t>Estructura básica implementada en Matlab del algoritmo.</t>
-  </si>
-  <si>
     <t>Integración del algoritmo de asociación de imágenes tipificadas con Matlab.</t>
   </si>
   <si>
     <t>Desarrollo de pruebas del algoritmo que determina la condición de un panel fotovoltaico a partir del análisis de imágenes termográficas.</t>
   </si>
   <si>
-    <t>Características de los escenarios más comunes donde se capturan imágenes termográficas a paneles fotovoltaicos.</t>
-  </si>
-  <si>
     <t>Establecer las condiciones de capturas de imágenes termográficas para la realización de pruebas con el algoritmos desarrollado.</t>
   </si>
   <si>
@@ -542,9 +494,6 @@
     <t>4.6. Documentación de hallazgos encontrados.</t>
   </si>
   <si>
-    <t>5. Ensayos y resultados.</t>
-  </si>
-  <si>
     <t>4. Implementación de algoritmo en Matlab.</t>
   </si>
   <si>
@@ -569,9 +518,6 @@
     <t>1.2. Desarrollo de pruebas de las técnicas de procesamiento de imágenes termográficas más comunes con Matlab.</t>
   </si>
   <si>
-    <t>5.1. Investigación sobre escenarios más comunes para la captura de imágenes termografica a paneles fotovoltaicos.</t>
-  </si>
-  <si>
     <t>5.2. Establecer las condiciones de capturas de imágenes termográficas para la realización de pruebas con el algoritmos desarrollado.</t>
   </si>
   <si>
@@ -590,9 +536,6 @@
     <t>10.000/h x 8h semanal x 40 semanas</t>
   </si>
   <si>
-    <t>Lista de imágenes con los tipos de daños o condiciones más frecuentes.</t>
-  </si>
-  <si>
     <t>6. Elaboración del documento, presentación.</t>
   </si>
   <si>
@@ -614,7 +557,76 @@
     <t>Implementar un algoritmo basado en técnicas de procesamiento de imágenes que determine la condición de un panel fotovoltaico a partir del análisis de imágenes termográficas.</t>
   </si>
   <si>
-    <t>Implementar escenarios de ensayo para verificar los resultados obtenidos.</t>
+    <t>Sección 1 del capitulo1: Técnicas de procesamiento de imágenes más comunes para identificar formas u objetos en imágenes termográficas de paneles fotovoltaicos.</t>
+  </si>
+  <si>
+    <t>Sección 2 del capitulo1: Listado sobre resultados de las técnicas más comunes.</t>
+  </si>
+  <si>
+    <t>Sección 3 del capitulo1: Selección de la técnica de procesamiento de imágenes adecuada para el proyecto.</t>
+  </si>
+  <si>
+    <t>Sección 2 del capitulo 2: Listado sobre tipos de daños o condiciones más frecuentes.</t>
+  </si>
+  <si>
+    <t>Sección 1 del capitulo 2: Tipos  de daños o condiciones observados en los paneles solares mediante imágenes termográficas.</t>
+  </si>
+  <si>
+    <t>Sección 3 del capitulo 2: Relación de las formas u objetos obtenidos en el procesamiento de imágenes termográficas en Matlab con el listado de tipos de daños o condiciones más frecuentes.</t>
+  </si>
+  <si>
+    <t>Sección 1 del capitulo 3: Definición almacenamiento de datos en Matlab.</t>
+  </si>
+  <si>
+    <t>Sección 2 del capitulo 3: Interface de los datos consultados por Matlab a la base de datos.</t>
+  </si>
+  <si>
+    <t>Sección 1 del capitulo 4: Modelo de algoritmo a construir en Matlab.</t>
+  </si>
+  <si>
+    <t>Sección 2 del capitulo 4:Determinación de condición de un panel fotovoltaico a partir de imagen termografica previamente verificada.</t>
+  </si>
+  <si>
+    <t>Evaluar el desempeño del algoritmo implementado bajo condiciones controladas.</t>
+  </si>
+  <si>
+    <t>Sección 1 capitulo 5: Procedimiento de captura imágenes termográficas a paneles fotovoltaicos para realizar la evaluación.</t>
+  </si>
+  <si>
+    <t>Sección 2 capitulo 5: Condiciones de captura de imágenes para la ejecución del algoritmo.</t>
+  </si>
+  <si>
+    <t>Sección 3 capitulo 5: Modelo de evaluación para el algoritmo desarrollado a partir de las condiciones de captura.</t>
+  </si>
+  <si>
+    <t>Sección 4 capitulo 5: Resultados de algoritmos; detección de condición de un panel fotovoltaico a parir de una imagen termográfica.</t>
+  </si>
+  <si>
+    <t>Sección 5 capitulo 5: Conclusión de la prueba realizada.</t>
+  </si>
+  <si>
+    <t>Módulo 1 del Algoritmo de análisis: Algoritmo de procesamiento de imágenes  termográficas en Matlab.</t>
+  </si>
+  <si>
+    <t>Módulo 2 del Algoritmo de análisis: Conjunto de imágenes almacenadas con los tipos de daños o condiciones más frecuentes.</t>
+  </si>
+  <si>
+    <t>Módulo 3 del Algoritmo de análisis: Algoritmo de asociación de imágenes tipificadas con Matlab.</t>
+  </si>
+  <si>
+    <t>Módulo 4 del Algoritmo de análisis: Estructura básica implementada en Matlab del algoritmo.</t>
+  </si>
+  <si>
+    <t>Módulo 4 del Algoritmo de análisis: Algoritmo de procesamiento de imágenes  termográficas en Matlab.</t>
+  </si>
+  <si>
+    <t>Módulo 4 del Algoritmo de análisis: Algoritmo capaz de obtener datos consultados de la base de datos.</t>
+  </si>
+  <si>
+    <t>Investigación sobre procedimiento de captura de imágenes termográficas que permita evaluar el desempeño del algoritmo.</t>
+  </si>
+  <si>
+    <t>5. Evaluación y resultados.</t>
   </si>
 </sst>
 </file>
@@ -2156,9 +2168,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2166,6 +2175,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5382,9 +5394,9 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5400,7 +5412,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B1" s="102"/>
       <c r="C1" s="102"/>
@@ -5423,9 +5435,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B3" s="75"/>
       <c r="C3" s="76" t="s">
@@ -5433,32 +5445,32 @@
       </c>
       <c r="D3" s="76"/>
       <c r="E3" s="76" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="104"/>
       <c r="B4" s="77"/>
       <c r="C4" s="76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="76"/>
       <c r="E4" s="76" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="104"/>
       <c r="B5" s="77"/>
       <c r="C5" s="78" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="78"/>
       <c r="E5" s="76" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="104"/>
       <c r="B6" s="77"/>
       <c r="C6" s="78" t="s">
@@ -5466,12 +5478,12 @@
       </c>
       <c r="D6" s="78"/>
       <c r="E6" s="78" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="103" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B7" s="75"/>
       <c r="C7" s="76" t="s">
@@ -5479,21 +5491,21 @@
       </c>
       <c r="D7" s="76"/>
       <c r="E7" s="76" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="104"/>
       <c r="B8" s="77"/>
       <c r="C8" s="76" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D8" s="76"/>
       <c r="E8" s="76" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="69" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="104"/>
       <c r="B9" s="77"/>
       <c r="C9" s="78" t="s">
@@ -5501,167 +5513,167 @@
       </c>
       <c r="D9" s="78"/>
       <c r="E9" s="78" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="103" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B10" s="75"/>
       <c r="C10" s="76" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D10" s="76"/>
       <c r="E10" s="76" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="104"/>
       <c r="B11" s="77"/>
       <c r="C11" s="76" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="D11" s="76"/>
       <c r="E11" s="76" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="104"/>
       <c r="B12" s="77"/>
       <c r="C12" s="76" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D12" s="76"/>
       <c r="E12" s="76" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="104"/>
       <c r="B13" s="77"/>
       <c r="C13" s="78" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D13" s="78"/>
       <c r="E13" s="78" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="103" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B14" s="75"/>
       <c r="C14" s="76" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D14" s="76"/>
       <c r="E14" s="76" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="104"/>
       <c r="B15" s="77"/>
       <c r="C15" s="76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D15" s="76"/>
       <c r="E15" s="78" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="104"/>
       <c r="B16" s="79"/>
       <c r="C16" s="76" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D16" s="76"/>
       <c r="E16" s="78" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="104"/>
       <c r="B17" s="79"/>
       <c r="C17" s="76" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D17" s="76"/>
       <c r="E17" s="76" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="104"/>
       <c r="B18" s="79"/>
       <c r="C18" s="76" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D18" s="76"/>
       <c r="E18" s="76" t="s">
-        <v>111</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="103" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B19" s="75"/>
       <c r="C19" s="76" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="D19" s="76"/>
       <c r="E19" s="76" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="104"/>
       <c r="B20" s="77"/>
       <c r="C20" s="76" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D20" s="76"/>
       <c r="E20" s="76" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="104"/>
       <c r="B21" s="79"/>
       <c r="C21" s="76" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D21" s="76"/>
       <c r="E21" s="78" t="s">
-        <v>115</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="104"/>
       <c r="B22" s="79"/>
       <c r="C22" s="76" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D22" s="76"/>
       <c r="E22" s="76" t="s">
-        <v>117</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="105"/>
       <c r="B23" s="80"/>
       <c r="C23" s="76" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D23" s="76"/>
       <c r="E23" s="76" t="s">
-        <v>119</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -5685,11 +5697,11 @@
   </sheetPr>
   <dimension ref="B1:AR105"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E75" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="AR105" sqref="B2:AR105"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:AR105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="45" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -5846,7 +5858,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="72">
@@ -6019,7 +6031,7 @@
     </row>
     <row r="9" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B9" s="112" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C9" s="113" t="s">
         <v>42</v>
@@ -6155,7 +6167,7 @@
     </row>
     <row r="12" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="107" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>42</v>
@@ -6291,7 +6303,7 @@
     </row>
     <row r="15" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B15" s="107" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C15" s="106" t="s">
         <v>42</v>
@@ -6427,7 +6439,7 @@
     </row>
     <row r="18" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B18" s="107" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C18" s="106" t="s">
         <v>42</v>
@@ -6563,7 +6575,7 @@
     </row>
     <row r="21" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B21" s="107" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C21" s="88" t="s">
         <v>41</v>
@@ -6743,7 +6755,7 @@
     </row>
     <row r="25" spans="2:44" s="12" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="118" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C25" s="119"/>
       <c r="E25" s="36"/>
@@ -6789,7 +6801,7 @@
     </row>
     <row r="26" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B26" s="84" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C26" s="88" t="s">
         <v>41</v>
@@ -6925,7 +6937,7 @@
     </row>
     <row r="29" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B29" s="84" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C29" s="88" t="s">
         <v>41</v>
@@ -7061,7 +7073,7 @@
     </row>
     <row r="32" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B32" s="84" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C32" s="88" t="s">
         <v>41</v>
@@ -7197,7 +7209,7 @@
     </row>
     <row r="35" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B35" s="84" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C35" s="88" t="s">
         <v>41</v>
@@ -7377,7 +7389,7 @@
     </row>
     <row r="39" spans="2:44" s="12" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="118" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C39" s="119"/>
       <c r="E39" s="26"/>
@@ -7423,7 +7435,7 @@
     </row>
     <row r="40" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B40" s="84" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C40" s="88" t="s">
         <v>41</v>
@@ -7559,7 +7571,7 @@
     </row>
     <row r="43" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B43" s="84" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C43" s="88" t="s">
         <v>42</v>
@@ -7695,7 +7707,7 @@
     </row>
     <row r="46" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B46" s="84" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C46" s="88" t="s">
         <v>42</v>
@@ -7787,7 +7799,7 @@
     </row>
     <row r="48" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B48" s="95"/>
-      <c r="C48" s="114"/>
+      <c r="C48" s="117"/>
       <c r="E48" s="24"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
@@ -7831,7 +7843,7 @@
     </row>
     <row r="49" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B49" s="84" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C49" s="88" t="s">
         <v>42</v>
@@ -7923,7 +7935,7 @@
     </row>
     <row r="51" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B51" s="95"/>
-      <c r="C51" s="114"/>
+      <c r="C51" s="117"/>
       <c r="E51" s="24"/>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
@@ -7967,9 +7979,9 @@
     </row>
     <row r="52" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B52" s="83" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="116" t="s">
         <v>41</v>
       </c>
       <c r="E52" s="21"/>
@@ -8147,7 +8159,7 @@
     </row>
     <row r="56" spans="2:44" s="12" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="110" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="C56" s="111"/>
       <c r="E56" s="26"/>
@@ -8193,7 +8205,7 @@
     </row>
     <row r="57" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B57" s="112" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C57" s="113" t="s">
         <v>42</v>
@@ -8329,7 +8341,7 @@
     </row>
     <row r="60" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B60" s="107" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C60" s="106" t="s">
         <v>42</v>
@@ -8465,7 +8477,7 @@
     </row>
     <row r="63" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B63" s="107" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C63" s="106" t="s">
         <v>42</v>
@@ -8601,7 +8613,7 @@
     </row>
     <row r="66" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B66" s="107" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C66" s="106" t="s">
         <v>42</v>
@@ -8737,7 +8749,7 @@
     </row>
     <row r="69" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B69" s="107" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C69" s="106" t="s">
         <v>41</v>
@@ -8873,7 +8885,7 @@
     </row>
     <row r="72" spans="2:44" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B72" s="107" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C72" s="106" t="s">
         <v>41</v>
@@ -9053,7 +9065,7 @@
     </row>
     <row r="76" spans="2:44" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="110" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="C76" s="111"/>
       <c r="E76" s="26"/>
@@ -9099,7 +9111,7 @@
     </row>
     <row r="77" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B77" s="112" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C77" s="113" t="s">
         <v>41</v>
@@ -9234,7 +9246,7 @@
     </row>
     <row r="80" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B80" s="107" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="C80" s="106" t="s">
         <v>42</v>
@@ -9370,7 +9382,7 @@
     </row>
     <row r="83" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B83" s="107" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C83" s="106" t="s">
         <v>42</v>
@@ -9506,7 +9518,7 @@
     </row>
     <row r="86" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B86" s="107" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C86" s="106" t="s">
         <v>42</v>
@@ -9642,7 +9654,7 @@
     </row>
     <row r="89" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B89" s="107" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="C89" s="106" t="s">
         <v>41</v>
@@ -9778,7 +9790,7 @@
     </row>
     <row r="92" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B92" s="107" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C92" s="106" t="s">
         <v>41</v>
@@ -9955,10 +9967,10 @@
       <c r="AR95" s="23"/>
     </row>
     <row r="96" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="115" t="s">
-        <v>170</v>
-      </c>
-      <c r="C96" s="116"/>
+      <c r="B96" s="114" t="s">
+        <v>151</v>
+      </c>
+      <c r="C96" s="115"/>
       <c r="E96" s="24"/>
       <c r="F96" s="18"/>
       <c r="G96" s="18"/>
@@ -10002,9 +10014,9 @@
     </row>
     <row r="97" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B97" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="C97" s="117" t="s">
+        <v>141</v>
+      </c>
+      <c r="C97" s="116" t="s">
         <v>41</v>
       </c>
       <c r="E97" s="26"/>
@@ -10138,7 +10150,7 @@
     </row>
     <row r="100" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B100" s="84" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C100" s="88" t="s">
         <v>42</v>
@@ -10274,7 +10286,7 @@
     </row>
     <row r="103" spans="2:44" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B103" s="84" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C103" s="88" t="s">
         <v>64</v>
@@ -10615,7 +10627,7 @@
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="66" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="F8" s="60">
         <v>1400000</v>
@@ -10640,7 +10652,7 @@
       </c>
       <c r="C9" s="67"/>
       <c r="D9" s="66" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="F9" s="60">
         <v>0</v>

</xml_diff>